<commit_message>
Admin access cmdlets 1
</commit_message>
<xml_diff>
--- a/docs/Tasks.xlsx
+++ b/docs/Tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="53">
   <si>
     <t>v3</t>
   </si>
   <si>
-    <t>Tests</t>
-  </si>
-  <si>
     <t>Help</t>
   </si>
   <si>
@@ -157,6 +154,30 @@
   </si>
   <si>
     <t>n/a</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Auto-Testing</t>
+  </si>
+  <si>
+    <t>_id alias</t>
+  </si>
+  <si>
+    <t>Invoke-McasRestMethod</t>
+  </si>
+  <si>
+    <t>Remove cmdlet alias</t>
+  </si>
+  <si>
+    <t>Credential only</t>
+  </si>
+  <si>
+    <t>Formatting</t>
+  </si>
+  <si>
+    <t>Error handling</t>
   </si>
 </sst>
 </file>
@@ -215,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -223,6 +244,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,382 +528,456 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="8.7265625" style="3"/>
+    <col min="3" max="5" width="13" style="3" customWidth="1"/>
+    <col min="6" max="6" width="22.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="13" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" t="s">
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>42</v>
-      </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H32">
+  <sortState ref="A2:O32">
     <sortCondition ref="B2:B32"/>
     <sortCondition ref="A2:A32"/>
   </sortState>

</xml_diff>

<commit_message>
Admin access cmdlets 3
</commit_message>
<xml_diff>
--- a/docs/Tasks.xlsx
+++ b/docs/Tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="54">
   <si>
     <t>v3</t>
   </si>
@@ -178,6 +178,10 @@
   </si>
   <si>
     <t>Error handling</t>
+  </si>
+  <si>
+    <t>Verbose
+Comments</t>
   </si>
 </sst>
 </file>
@@ -528,11 +532,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I6" sqref="I6"/>
+      <selection pane="topRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,10 +547,10 @@
     <col min="6" max="6" width="22.36328125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="15" width="13" style="3" customWidth="1"/>
+    <col min="9" max="16" width="13" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -577,23 +581,26 @@
       <c r="J1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -625,7 +632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -641,11 +648,11 @@
       <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -677,7 +684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -693,11 +700,11 @@
       <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -705,7 +712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -713,7 +720,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -721,7 +728,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -729,7 +736,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -745,11 +752,11 @@
       <c r="E10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L10" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -757,7 +764,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -765,7 +772,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -773,7 +780,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -781,7 +788,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -789,7 +796,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -797,7 +804,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -805,7 +812,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -821,11 +828,11 @@
       <c r="E18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L18" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -833,7 +840,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -841,7 +848,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -849,7 +856,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -857,7 +864,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -865,7 +872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -873,7 +880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -889,11 +896,11 @@
       <c r="E25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L25" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -901,7 +908,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -917,11 +924,11 @@
       <c r="E27" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K27" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L27" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -937,14 +944,14 @@
       <c r="E28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N28" s="3" t="s">
+      <c r="L28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O28" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -952,7 +959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -960,7 +967,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -968,7 +975,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -977,7 +984,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:O32">
+  <sortState ref="A2:P32">
     <sortCondition ref="B2:B32"/>
     <sortCondition ref="A2:A32"/>
   </sortState>

</xml_diff>

<commit_message>
Get-MCASAlert added to v3
</commit_message>
<xml_diff>
--- a/docs/Tasks.xlsx
+++ b/docs/Tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="54">
   <si>
     <t>v3</t>
   </si>
@@ -534,9 +534,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -907,6 +907,9 @@
       <c r="B26" t="s">
         <v>9</v>
       </c>
+      <c r="C26" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" t="s">

</xml_diff>

<commit_message>
Get-MCASAlert #1 with revisions to Invoke-MCASRestMethod
</commit_message>
<xml_diff>
--- a/docs/Tasks.xlsx
+++ b/docs/Tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="54">
   <si>
     <t>v3</t>
   </si>
@@ -205,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +215,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -240,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -251,6 +257,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,11 +542,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D26" sqref="D26"/>
+      <selection pane="topRight" activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,10 +557,10 @@
     <col min="6" max="6" width="22.36328125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16" width="13" style="3" customWidth="1"/>
+    <col min="9" max="17" width="13" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -581,26 +591,27 @@
       <c r="J1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2"/>
+      <c r="L1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -632,7 +643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -648,11 +659,11 @@
       <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="M3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -684,7 +695,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -700,11 +711,11 @@
       <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="M5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -712,7 +723,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -720,7 +731,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -728,7 +739,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -736,7 +747,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -752,11 +763,11 @@
       <c r="E10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="M10" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -764,7 +775,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -772,7 +783,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -780,7 +791,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -788,7 +799,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -796,7 +807,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -804,7 +815,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -812,7 +823,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -828,11 +839,11 @@
       <c r="E18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L18" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M18" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -840,7 +851,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -848,7 +859,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -856,7 +867,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -864,7 +875,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -872,7 +883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -880,7 +891,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -896,22 +907,50 @@
       <c r="E25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L25" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="M25" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -927,11 +966,11 @@
       <c r="E27" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L27" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M27" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -947,14 +986,14 @@
       <c r="E28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O28" s="3" t="s">
+      <c r="M28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P28" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -962,7 +1001,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -970,7 +1009,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -978,7 +1017,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -987,7 +1026,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:P32">
+  <sortState ref="A2:Q32">
     <sortCondition ref="B2:B32"/>
     <sortCondition ref="A2:A32"/>
   </sortState>

</xml_diff>

<commit_message>
Get-MCASActivity and ConvertFrom-MCASTimestamp functional an
</commit_message>
<xml_diff>
--- a/docs/Tasks.xlsx
+++ b/docs/Tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="55">
   <si>
     <t>v3</t>
   </si>
@@ -549,7 +549,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K28" sqref="K28"/>
+      <selection pane="topRight" activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -886,12 +886,47 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="24" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
         <v>9</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">
@@ -948,10 +983,16 @@
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
+      <c r="N26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
+      <c r="Q26" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">

</xml_diff>

<commit_message>
Set-MCASIPRangeSet not yet ready
</commit_message>
<xml_diff>
--- a/docs/Tasks.xlsx
+++ b/docs/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A859CB27-6B60-44DC-AB9D-568B7AF3A7C0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC754F6D-E629-44F0-BE88-BEEBB4110E91}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="58">
   <si>
     <t>v3</t>
   </si>
@@ -119,12 +119,6 @@
   </si>
   <si>
     <t>Data Enrichment</t>
-  </si>
-  <si>
-    <t>Set-MCASIPRange</t>
-  </si>
-  <si>
-    <t>Remove-MCASIPRange</t>
   </si>
   <si>
     <t>Get-MCASUserGroup</t>
@@ -192,13 +186,22 @@
   </si>
   <si>
     <t>Get-MCASIPRangeSet</t>
+  </si>
+  <si>
+    <t>Set-MCASIPRangeSet</t>
+  </si>
+  <si>
+    <t>Remove-MCASIPRangeSet</t>
+  </si>
+  <si>
+    <t>Other Pipelining</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,8 +217,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,6 +242,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -253,10 +268,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -268,21 +284,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -569,11 +579,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A9" sqref="A9"/>
+      <selection pane="topRight" activeCell="D13" sqref="D13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -586,11 +596,12 @@
     <col min="8" max="8" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16" width="13" style="1" customWidth="1"/>
     <col min="17" max="17" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="4" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>7</v>
@@ -605,43 +616,46 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="K1" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -676,12 +690,12 @@
         <v>6</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -717,10 +731,10 @@
         <v>6</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -755,10 +769,10 @@
         <v>6</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -796,10 +810,10 @@
         <v>6</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -843,7 +857,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -882,7 +896,7 @@
       </c>
       <c r="P7"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -917,12 +931,12 @@
         <v>6</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
         <v>32</v>
@@ -957,10 +971,13 @@
       <c r="M9" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>32</v>
@@ -992,16 +1009,19 @@
       <c r="K10" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="L10" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="M10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
@@ -1030,22 +1050,10 @@
       <c r="J11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>55</v>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>54</v>
       </c>
       <c r="B12" t="s">
         <v>32</v>
@@ -1074,26 +1082,53 @@
       <c r="J12" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>34</v>
+      <c r="K12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="B13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
         <v>23</v>
@@ -1126,11 +1161,11 @@
         <v>6</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P15"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1171,10 +1206,10 @@
         <v>6</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>6</v>
@@ -1192,7 +1227,7 @@
         <v>6</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>6</v>
@@ -1321,7 +1356,7 @@
         <v>6</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
@@ -1383,10 +1418,10 @@
         <v>6</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>6</v>
@@ -1395,7 +1430,7 @@
         <v>6</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>6</v>
@@ -1404,12 +1439,12 @@
         <v>6</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
         <v>9</v>
@@ -1459,7 +1494,7 @@
         <v>6</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
@@ -1480,7 +1515,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
         <v>9</v>
@@ -1513,23 +1548,23 @@
         <v>6</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1537,13 +1572,8 @@
     <sortCondition ref="B2:B35"/>
     <sortCondition ref="A2:A35"/>
   </sortState>
-  <conditionalFormatting sqref="C37:P1048576 C1:P35">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"x"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="C37:P1048576 C13:P35 Q13:Q1048576 C1:Q12">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added Get-MCASStream and Get-MCASDiscoveredApp
</commit_message>
<xml_diff>
--- a/docs/Tasks.xlsx
+++ b/docs/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660537E9-64F5-495B-A9E9-A154354F8D46}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D07E43-9700-4BDE-838E-DE52A38F633B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="59">
   <si>
     <t>v3</t>
   </si>
@@ -594,7 +594,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A16" sqref="A16"/>
+      <selection pane="topRight" activeCell="A16" sqref="A16:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -602,10 +602,13 @@
     <col min="1" max="1" width="31.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="13" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16" width="13" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="13" style="1" customWidth="1"/>
     <col min="17" max="17" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.08984375" bestFit="1" customWidth="1"/>
   </cols>
@@ -627,16 +630,16 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>43</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>44</v>
@@ -1265,6 +1268,39 @@
       <c r="B17" t="s">
         <v>23</v>
       </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -1291,7 +1327,7 @@
         <v>6</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>38</v>
@@ -1300,7 +1336,7 @@
         <v>6</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>6</v>
@@ -1325,6 +1361,39 @@
       <c r="B20" t="s">
         <v>23</v>
       </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -1503,7 +1572,7 @@
         <v>6</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>38</v>
@@ -1512,7 +1581,7 @@
         <v>6</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>38</v>
@@ -1657,7 +1726,7 @@
     <sortCondition ref="B2:B35"/>
     <sortCondition ref="A2:A35"/>
   </sortState>
-  <conditionalFormatting sqref="C37:P1048576 C13:P35 C1:Q12 Q13:Q1048576">
+  <conditionalFormatting sqref="Q13:Q1048576 C37:P1048576 J13:P35 J1:Q12 C1:I35">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>

</xml_diff>

<commit_message>
cleanup old commented code
</commit_message>
<xml_diff>
--- a/docs/Tasks.xlsx
+++ b/docs/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62331B43-D47A-4019-877D-70F6DFEB3212}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951F8556-4CCA-47D1-9120-71959CB111E2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="60">
   <si>
     <t>v3</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>from Get-MCASAppId</t>
+  </si>
+  <si>
+    <t>ConvertFrom-MCASTimestamp</t>
   </si>
 </sst>
 </file>
@@ -235,7 +238,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +259,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -282,7 +291,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -297,6 +306,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -590,11 +601,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A22" sqref="A22"/>
+      <selection pane="topRight" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -670,7 +681,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B2" t="s">
@@ -708,7 +719,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B3" t="s">
@@ -749,7 +760,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
@@ -787,7 +798,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B5" t="s">
@@ -872,7 +883,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
@@ -949,7 +960,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B9" t="s">
@@ -990,7 +1001,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B10" t="s">
@@ -1034,7 +1045,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B11" t="s">
@@ -1066,7 +1077,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B12" t="s">
@@ -1104,7 +1115,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B13" t="s">
@@ -1134,7 +1145,7 @@
       <c r="R13" s="3"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B14" t="s">
@@ -1303,7 +1314,7 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B18" t="s">
@@ -1341,7 +1352,7 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B19" t="s">
@@ -1566,7 +1577,7 @@
       <c r="P25"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="A26" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B26" t="s">
@@ -1690,7 +1701,7 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="A29" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B29" t="s">
@@ -1761,7 +1772,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="A33" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B33" t="s">
@@ -1812,6 +1823,14 @@
       </c>
       <c r="B35" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get-Report and Get-ReportContent functional with pipelining
</commit_message>
<xml_diff>
--- a/docs/Tasks.xlsx
+++ b/docs/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E217B212-8E44-4597-A032-1903844B4CCE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AAB0A4-482D-4F79-85B6-958D5741D3E3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="73">
   <si>
     <t>v3</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t>Import-MCASDynamicData</t>
+  </si>
+  <si>
+    <t>to Get-MCASReportContent</t>
+  </si>
+  <si>
+    <t>from Get-MCASReport</t>
   </si>
 </sst>
 </file>
@@ -694,7 +700,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A44" sqref="A44"/>
+      <selection pane="topRight" activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -711,7 +717,7 @@
     <col min="12" max="12" width="15.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="17" width="13" style="1" customWidth="1"/>
     <col min="18" max="18" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="45.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1688,7 +1694,7 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
+      <c r="A23" t="s">
         <v>35</v>
       </c>
       <c r="B23" t="s">
@@ -1718,10 +1724,21 @@
       <c r="K23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L23" s="5"/>
+      <c r="L23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S23" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
+      <c r="A24" t="s">
         <v>59</v>
       </c>
       <c r="B24" t="s">
@@ -1751,9 +1768,17 @@
       <c r="K24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L24" s="5"/>
+      <c r="L24" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="M24" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S24" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.35">

</xml_diff>